<commit_message>
Reto2: Update Cavas file
</commit_message>
<xml_diff>
--- a/Reto2/Scio - Modelo de Negocios.xlsx
+++ b/Reto2/Scio - Modelo de Negocios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\UNIVERSIDAD\POSGRADO\Moviles\movilesunal2020\Reto2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBF2AF7-8D2D-422D-BD49-9841A4E04C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C65336-70A7-4B22-854B-7CB57105F1F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1620,6 +1620,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,9 +1645,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2175,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="78" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2191,14 +2191,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2220,47 +2220,47 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+    <row r="2" spans="1:26" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="101"/>
+      <c r="D2" s="102"/>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="99" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="186" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
+      <c r="A3" s="100"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="104"/>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="99"/>
+      <c r="F3" s="100"/>
     </row>
     <row r="4" spans="1:26" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="105" t="s">
+      <c r="B4" s="97"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="96"/>
-      <c r="F4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="98"/>
     </row>
     <row r="5" spans="1:26" ht="342.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="342.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3276,7 +3276,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3534,10 +3536,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="97"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="1"/>
@@ -4674,8 +4676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AL1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4686,46 +4688,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96"/>
-      <c r="AC1" s="96"/>
-      <c r="AD1" s="96"/>
-      <c r="AE1" s="96"/>
-      <c r="AF1" s="96"/>
-      <c r="AG1" s="96"/>
-      <c r="AH1" s="96"/>
-      <c r="AI1" s="96"/>
-      <c r="AJ1" s="96"/>
-      <c r="AK1" s="96"/>
-      <c r="AL1" s="97"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="98"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>

</xml_diff>